<commit_message>
issue #5: stock data output to json file
</commit_message>
<xml_diff>
--- a/legislator/property/output/normal/丁守中_2011-11-22_財產申報表_tmp8fef1.xlsx
+++ b/legislator/property/output/normal/丁守中_2011-11-22_財產申報表_tmp8fef1.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="126">
   <si>
     <t>土地坐落</t>
   </si>
@@ -237,6 +237,9 @@
     <t>total</t>
   </si>
   <si>
+    <t>property_category</t>
+  </si>
+  <si>
     <t>date</t>
   </si>
   <si>
@@ -261,13 +264,16 @@
     <t>元晶太陽能股份有限公司</t>
   </si>
   <si>
-    <t>旭晶能源科技股份有限公 司</t>
-  </si>
-  <si>
-    <t>珀碩聯.合科技股份有限公 司</t>
-  </si>
-  <si>
-    <t>景岳生物科技股份有限公 司</t>
+    <t>旭晶能源科技股份有限公司</t>
+  </si>
+  <si>
+    <t>珀碩聯.合科技股份有限公司</t>
+  </si>
+  <si>
+    <t>景岳生物科技股份有限公司</t>
+  </si>
+  <si>
+    <t>stock</t>
   </si>
   <si>
     <t>2011-11-22</t>
@@ -1448,13 +1454,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="B1" s="1" t="s">
         <v>65</v>
       </c>
@@ -1482,13 +1488,16 @@
       <c r="J1" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>81</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>15</v>
@@ -1506,16 +1515,19 @@
         <v>16445990</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="2">
+        <v>84</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="2">
         <v>515</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>82</v>
       </c>
@@ -1538,21 +1550,24 @@
         <v>700000</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="2">
+        <v>84</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="2">
         <v>515</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="A4" s="1">
         <v>83</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>15</v>
@@ -1570,21 +1585,24 @@
         <v>500000</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="2">
+        <v>84</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="2">
         <v>515</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5" s="1">
         <v>84</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>14</v>
@@ -1602,21 +1620,24 @@
         <v>2400000</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="2">
+        <v>84</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="2">
         <v>515</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>85</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>14</v>
@@ -1634,21 +1655,24 @@
         <v>312740</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="2">
+        <v>84</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="2">
         <v>515</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7" s="1">
         <v>86</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>15</v>
@@ -1666,21 +1690,24 @@
         <v>2500000</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="2">
+        <v>84</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="2">
         <v>515</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8" s="1">
         <v>87</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>14</v>
@@ -1698,21 +1725,24 @@
         <v>2000000</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="2">
+        <v>84</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="2">
         <v>515</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9" s="1">
         <v>88</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>14</v>
@@ -1730,21 +1760,24 @@
         <v>1150000</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="2">
+        <v>84</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="2">
         <v>515</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10" s="1">
         <v>89</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>15</v>
@@ -1762,21 +1795,24 @@
         <v>400000</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="2">
+        <v>84</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="2">
         <v>515</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11" s="1">
         <v>90</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>15</v>
@@ -1794,12 +1830,15 @@
         <v>480000</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J11" s="2">
+        <v>84</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="2">
         <v>515</v>
       </c>
     </row>
@@ -1818,16 +1857,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1835,7 +1874,7 @@
         <v>110</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C2" s="2">
         <v>2</v>
@@ -1852,7 +1891,7 @@
         <v>111</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C3" s="2">
         <v>3</v>
@@ -1879,16 +1918,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1896,16 +1935,16 @@
         <v>116</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1913,16 +1952,16 @@
         <v>117</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1930,16 +1969,16 @@
         <v>118</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1947,16 +1986,16 @@
         <v>119</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1964,16 +2003,16 @@
         <v>120</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1994,19 +2033,19 @@
         <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2014,22 +2053,22 @@
         <v>130</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E2" s="2">
         <v>21113089</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2037,22 +2076,22 @@
         <v>131</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E3" s="2">
         <v>9650048</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2070,22 +2109,22 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2096,19 +2135,19 @@
         <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E2" s="2">
         <v>990000</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2119,19 +2158,19 @@
         <v>64</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E3" s="2">
         <v>2940000</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
issue #5: stock data from json to db
</commit_message>
<xml_diff>
--- a/legislator/property/output/normal/丁守中_2011-11-22_財產申報表_tmp8fef1.xlsx
+++ b/legislator/property/output/normal/丁守中_2011-11-22_財產申報表_tmp8fef1.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="131">
   <si>
     <t>土地坐落</t>
   </si>
@@ -240,6 +240,9 @@
     <t>property_category</t>
   </si>
   <si>
+    <t>category</t>
+  </si>
+  <si>
     <t>date</t>
   </si>
   <si>
@@ -249,6 +252,12 @@
     <t>legislator_id</t>
   </si>
   <si>
+    <t>source_file</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
     <t>琉園股份有限公司</t>
   </si>
   <si>
@@ -276,7 +285,13 @@
     <t>stock</t>
   </si>
   <si>
+    <t>normal</t>
+  </si>
+  <si>
     <t>2011-11-22</t>
+  </si>
+  <si>
+    <t>tmp8fef1</t>
   </si>
   <si>
     <t>財產種類</t>
@@ -1454,13 +1469,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:14">
       <c r="B1" s="1" t="s">
         <v>65</v>
       </c>
@@ -1491,13 +1506,22 @@
       <c r="K1" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="1">
         <v>81</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>15</v>
@@ -1515,19 +1539,28 @@
         <v>16445990</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="2">
+        <v>88</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="2">
         <v>515</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="M2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="N2" s="2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="1">
         <v>82</v>
       </c>
@@ -1550,24 +1583,33 @@
         <v>700000</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="2">
+        <v>88</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="2">
         <v>515</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="M3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="N3" s="2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="1">
         <v>83</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>15</v>
@@ -1585,24 +1627,33 @@
         <v>500000</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="2">
+        <v>515</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="N4" s="2">
         <v>83</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="2">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="1">
         <v>84</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>14</v>
@@ -1620,24 +1671,33 @@
         <v>2400000</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I5" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="2">
+        <v>515</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="N5" s="2">
         <v>84</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" s="2">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="1">
         <v>85</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>14</v>
@@ -1655,24 +1715,33 @@
         <v>312740</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K6" s="2">
+        <v>88</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="2">
         <v>515</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="M6" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="N6" s="2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="1">
         <v>86</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>15</v>
@@ -1690,24 +1759,33 @@
         <v>2500000</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="2">
+        <v>88</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="2">
         <v>515</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="M7" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="N7" s="2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="1">
         <v>87</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>14</v>
@@ -1725,24 +1803,33 @@
         <v>2000000</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" s="2">
+        <v>88</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="2">
         <v>515</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="M8" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="N8" s="2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="1">
         <v>88</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>14</v>
@@ -1760,24 +1847,33 @@
         <v>1150000</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K9" s="2">
+        <v>88</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" s="2">
         <v>515</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="M9" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="N9" s="2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="1">
         <v>89</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>15</v>
@@ -1795,24 +1891,33 @@
         <v>400000</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K10" s="2">
+        <v>88</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="2">
         <v>515</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="M10" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="N10" s="2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="1">
         <v>90</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>15</v>
@@ -1830,16 +1935,25 @@
         <v>480000</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="2">
+        <v>88</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="2">
         <v>515</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="N11" s="2">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1857,16 +1971,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1874,7 +1988,7 @@
         <v>110</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C2" s="2">
         <v>2</v>
@@ -1891,7 +2005,7 @@
         <v>111</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C3" s="2">
         <v>3</v>
@@ -1918,16 +2032,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1935,16 +2049,16 @@
         <v>116</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1952,16 +2066,16 @@
         <v>117</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1969,16 +2083,16 @@
         <v>118</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1986,16 +2100,16 @@
         <v>119</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2003,16 +2117,16 @@
         <v>120</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2033,19 +2147,19 @@
         <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2053,22 +2167,22 @@
         <v>130</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E2" s="2">
         <v>21113089</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2076,22 +2190,22 @@
         <v>131</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E3" s="2">
         <v>9650048</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2109,22 +2223,22 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2135,19 +2249,19 @@
         <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="E2" s="2">
         <v>990000</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2158,19 +2272,19 @@
         <v>64</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="E3" s="2">
         <v>2940000</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
issue #5: property land done
</commit_message>
<xml_diff>
--- a/legislator/property/output/normal/丁守中_2011-11-22_財產申報表_tmp8fef1.xlsx
+++ b/legislator/property/output/normal/丁守中_2011-11-22_財產申報表_tmp8fef1.xlsx
@@ -22,9 +22,114 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="131">
-  <si>
-    <t>土地坐落</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="131">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>share_portion</t>
+  </si>
+  <si>
+    <t>owner</t>
+  </si>
+  <si>
+    <t>register_date</t>
+  </si>
+  <si>
+    <t>register_reason</t>
+  </si>
+  <si>
+    <t>acquire_value</t>
+  </si>
+  <si>
+    <t>property_category</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>legislator_name</t>
+  </si>
+  <si>
+    <t>legislator_id</t>
+  </si>
+  <si>
+    <t>source_file</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>臺北市北投區振興段一小段00930000地號</t>
+  </si>
+  <si>
+    <t>臺北市北投區振興段一小段00660000地號</t>
+  </si>
+  <si>
+    <t>臺北市北投區湖田段二小段00210008地號</t>
+  </si>
+  <si>
+    <t>10000分之101</t>
+  </si>
+  <si>
+    <t>97300分之4170</t>
+  </si>
+  <si>
+    <t>10000分之84</t>
+  </si>
+  <si>
+    <t>全部</t>
+  </si>
+  <si>
+    <t>丁守中</t>
+  </si>
+  <si>
+    <t>溫子苓</t>
+  </si>
+  <si>
+    <t>78年10月11曰</t>
+  </si>
+  <si>
+    <t>93年08月19日</t>
+  </si>
+  <si>
+    <t>85年05月24日</t>
+  </si>
+  <si>
+    <t>97.年07月22日</t>
+  </si>
+  <si>
+    <t>買賣</t>
+  </si>
+  <si>
+    <t>繼承</t>
+  </si>
+  <si>
+    <t>(超過五年）</t>
+  </si>
+  <si>
+    <t>(2970萬元）</t>
+  </si>
+  <si>
+    <t>land</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>2011-11-22</t>
+  </si>
+  <si>
+    <t>tmp8fef1</t>
+  </si>
+  <si>
+    <t>建物標示</t>
   </si>
   <si>
     <t>面積（平方公尺）</t>
@@ -36,115 +141,58 @@
     <t>所有權人</t>
   </si>
   <si>
+    <t>登記（取得\時間</t>
+  </si>
+  <si>
+    <t>登記（取得）原因</t>
+  </si>
+  <si>
+    <t>取得價額</t>
+  </si>
+  <si>
+    <t>臺北市北投區振興段一小段12407000建號（（陽台20.87平方公尺)）</t>
+  </si>
+  <si>
+    <t>臺北市北投區振興段一小段12496000建號（（地下室停車位)）</t>
+  </si>
+  <si>
+    <t>臺北市北投區振興段一小段12398000建號（（陽台12.5平方公尺)）</t>
+  </si>
+  <si>
+    <t>臺北市北投區振興段一小段12884000建號(（陽台13.10平</t>
+  </si>
+  <si>
+    <t>臺北市北投區振興段一小段12891000建號（（地下室停車位））</t>
+  </si>
+  <si>
+    <t>56分之1</t>
+  </si>
+  <si>
+    <t>100000分之4464</t>
+  </si>
+  <si>
+    <t>93年08月</t>
+  </si>
+  <si>
+    <t>93年08月19曰</t>
+  </si>
+  <si>
+    <t>廠牌型號</t>
+  </si>
+  <si>
+    <t>汽缸容量</t>
+  </si>
+  <si>
+    <t>所有A</t>
+  </si>
+  <si>
     <t>登記（取得）時間</t>
   </si>
   <si>
-    <t>登記（取得）原因</t>
-  </si>
-  <si>
-    <t>取得價額</t>
-  </si>
-  <si>
-    <t>臺北市北投區振興段一小段 0093-0000 地號</t>
-  </si>
-  <si>
-    <t>臺北市北投區振興段一小段 0066-0000 地號</t>
-  </si>
-  <si>
-    <t>臺北市北投區湖田段二小段 0021-0008 地號</t>
-  </si>
-  <si>
-    <t>10000分之 101</t>
-  </si>
-  <si>
-    <t>97300分之 4170</t>
-  </si>
-  <si>
-    <t>10000分之 84</t>
-  </si>
-  <si>
-    <t>全部</t>
-  </si>
-  <si>
-    <t>丁守中</t>
-  </si>
-  <si>
-    <t>溫子苓</t>
-  </si>
-  <si>
-    <t>78年10月 11曰</t>
-  </si>
-  <si>
-    <t>93年08月 19日</t>
-  </si>
-  <si>
-    <t>85年05月 24日</t>
-  </si>
-  <si>
-    <t>97.年07月 22日</t>
-  </si>
-  <si>
-    <t>買賣</t>
-  </si>
-  <si>
-    <t>繼承</t>
-  </si>
-  <si>
-    <t>(超過五年）</t>
-  </si>
-  <si>
-    <t>(2970萬元）</t>
-  </si>
-  <si>
-    <t>建物標示</t>
-  </si>
-  <si>
-    <t>登記（取得\時間</t>
-  </si>
-  <si>
-    <t>臺北市北投區振興段一小段 12407-000 建號（（陽台 20.87 平 方公尺)）</t>
-  </si>
-  <si>
-    <t>臺北市北投區振興段一小段 12496-000建號（（地下室停車 位)）</t>
-  </si>
-  <si>
-    <t>臺北市北投區振興段一小段 12398-000建號（（陽台12.5平 方公尺)）</t>
-  </si>
-  <si>
-    <t>臺北市北投區振興段一小段 12884-000 建號(（陽台 13.10 平</t>
-  </si>
-  <si>
-    <t>臺北市北投區振興段一小段 12891-000建號（（地下室停車 位））</t>
-  </si>
-  <si>
-    <t>56分之1</t>
-  </si>
-  <si>
-    <t>100000 分 之 4464</t>
-  </si>
-  <si>
-    <t>85年05月' 24日</t>
-  </si>
-  <si>
-    <t>93年08月</t>
-  </si>
-  <si>
-    <t>93年08月 19曰</t>
-  </si>
-  <si>
-    <t>廠牌型號</t>
-  </si>
-  <si>
-    <t>汽缸容量</t>
-  </si>
-  <si>
-    <t>所有A</t>
-  </si>
-  <si>
-    <t>LEXUS ES350</t>
-  </si>
-  <si>
-    <t>100 年 04 月19曰</t>
+    <t>LEXUSES350</t>
+  </si>
+  <si>
+    <t>100年04月19曰</t>
   </si>
   <si>
     <t>貝賣</t>
@@ -186,7 +234,7 @@
     <t>華南商業銀行信託部</t>
   </si>
   <si>
-    <t>兆豐國際商業銀行總管理 處</t>
+    <t>兆豐國際商業銀行總管理處</t>
   </si>
   <si>
     <t>活期儲蓄存款</t>
@@ -201,30 +249,18 @@
     <t>支票存款</t>
   </si>
   <si>
-    <t>活期儲蓄存款'</t>
-  </si>
-  <si>
     <t>新臺幣</t>
   </si>
   <si>
-    <t>新臺幣 t</t>
+    <t>新臺幣t</t>
   </si>
   <si>
     <t>美金</t>
   </si>
   <si>
-    <t>新臺幣 -</t>
-  </si>
-  <si>
     <t>丁〇豪</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>owner</t>
-  </si>
-  <si>
     <t>quantity</t>
   </si>
   <si>
@@ -237,27 +273,6 @@
     <t>total</t>
   </si>
   <si>
-    <t>property_category</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>legislator_name</t>
-  </si>
-  <si>
-    <t>legislator_id</t>
-  </si>
-  <si>
-    <t>source_file</t>
-  </si>
-  <si>
-    <t>index</t>
-  </si>
-  <si>
     <t>琉園股份有限公司</t>
   </si>
   <si>
@@ -285,19 +300,10 @@
     <t>stock</t>
   </si>
   <si>
-    <t>normal</t>
-  </si>
-  <si>
-    <t>2011-11-22</t>
-  </si>
-  <si>
-    <t>tmp8fef1</t>
-  </si>
-  <si>
     <t>財產種類</t>
   </si>
   <si>
-    <t>項/件</t>
+    <t>項件</t>
   </si>
   <si>
     <t>價額</t>
@@ -306,7 +312,7 @@
     <t>手錶</t>
   </si>
   <si>
-    <t>手錶’珠寶 ■</t>
+    <t>手錶珠寶■</t>
   </si>
   <si>
     <t>保險公司</t>
@@ -330,31 +336,31 @@
     <t>國泰人壽</t>
   </si>
   <si>
-    <t>南山康福2 0年期終身壽險</t>
+    <t>南山康福20年期終身壽險</t>
   </si>
   <si>
     <t>終身壽險</t>
   </si>
   <si>
-    <t>2 0年期年繳6 8 3 1 0 元 .</t>
-  </si>
-  <si>
-    <t>2 t)年期终身壽險年繳5 6 1 6 7元</t>
-  </si>
-  <si>
-    <t>新2 0年期繳費特別增值分 红年繳6 4 6 0 2元</t>
-  </si>
-  <si>
-    <t>新2b年繳費特別增值分紅 年繳41542元</t>
-  </si>
-  <si>
-    <t>终身壽險年繳5 5 4 0 7 元</t>
+    <t>20年期年繳68310元.</t>
+  </si>
+  <si>
+    <t>2t)年期终身壽險年繳56167元</t>
+  </si>
+  <si>
+    <t>新20年期繳費特別增值分红年繳64602元</t>
+  </si>
+  <si>
+    <t>新2b年繳費特別增值分紅年繳41542元</t>
+  </si>
+  <si>
+    <t>终身壽險年繳55407元</t>
   </si>
   <si>
     <t>債務人</t>
   </si>
   <si>
-    <t>債權人及•地址</t>
+    <t>債權人及地址</t>
   </si>
   <si>
     <t>餘額</t>
@@ -372,16 +378,13 @@
     <t>房岸十地抵押貸款</t>
   </si>
   <si>
-    <t>華南銀行 臺北市北投區北投路</t>
-  </si>
-  <si>
-    <t>100年01月 10日</t>
-  </si>
-  <si>
-    <t>房屋土地抵 押貸款 '</t>
-  </si>
-  <si>
-    <t>房屋土地抵 押貸款</t>
+    <t>華南銀行臺北市北投區北投路</t>
+  </si>
+  <si>
+    <t>100年01月10日</t>
+  </si>
+  <si>
+    <t>房屋土地抵押貸款</t>
   </si>
   <si>
     <t>投資人</t>
@@ -396,19 +399,16 @@
     <t>投資金額</t>
   </si>
   <si>
-    <t>_取得（發生）時間</t>
-  </si>
-  <si>
     <t>鼎天股份有限公司</t>
   </si>
   <si>
-    <t>臺北市北投路二段13號10 樓之一</t>
-  </si>
-  <si>
-    <t>95年09月 01日</t>
-  </si>
-  <si>
-    <t>97年02月 01日</t>
+    <t>臺北市北投路二段13號10樓之一</t>
+  </si>
+  <si>
+    <t>95年09月01日</t>
+  </si>
+  <si>
+    <t>97年02月01日</t>
   </si>
   <si>
     <t>投資</t>
@@ -773,13 +773,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:15">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -801,109 +801,214 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="1">
         <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2">
         <v>3971</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="2">
+        <v>515</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="2">
         <v>14</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="1">
         <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2">
         <v>973</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>29</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="2">
+        <v>515</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="1">
         <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2">
         <v>3971</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>29</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="2">
+        <v>515</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="1">
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2">
         <v>2975.21</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="2">
+        <v>515</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O5" s="2">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -921,25 +1026,25 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -947,25 +1052,25 @@
         <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2">
         <v>193.66</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -973,25 +1078,25 @@
         <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="C3" s="2">
         <v>2357.46</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -999,25 +1104,25 @@
         <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C4" s="2">
         <v>153.32</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1025,25 +1130,25 @@
         <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="C5" s="2">
         <v>2357.46</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1051,25 +1156,25 @@
         <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C6" s="2">
         <v>126.18</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1077,25 +1182,25 @@
         <v>32</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="C7" s="2">
         <v>1350.27</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1113,22 +1218,22 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1136,19 +1241,19 @@
         <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="C2" s="2">
         <v>3456</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="G2" s="2">
         <v>600000</v>
@@ -1169,22 +1274,22 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1192,16 +1297,16 @@
         <v>61</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2">
@@ -1213,16 +1318,16 @@
         <v>62</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2">
@@ -1234,16 +1339,16 @@
         <v>63</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2">
@@ -1255,16 +1360,16 @@
         <v>64</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2">
@@ -1276,16 +1381,16 @@
         <v>65</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2">
@@ -1297,16 +1402,16 @@
         <v>66</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2">
         <v>20468.96</v>
@@ -1320,16 +1425,16 @@
         <v>67</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2">
@@ -1341,16 +1446,16 @@
         <v>68</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2">
@@ -1362,16 +1467,16 @@
         <v>70</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2">
@@ -1383,16 +1488,16 @@
         <v>71</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2">
@@ -1404,16 +1509,16 @@
         <v>72</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2">
@@ -1425,16 +1530,16 @@
         <v>73</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2">
@@ -1446,16 +1551,16 @@
         <v>74</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2">
@@ -1477,43 +1582,43 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>73</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>77</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -1521,10 +1626,10 @@
         <v>81</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D2" s="2">
         <v>1644599</v>
@@ -1533,28 +1638,28 @@
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="G2" s="2">
         <v>16445990</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="L2" s="2">
         <v>515</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="N2" s="2">
         <v>81</v>
@@ -1565,10 +1670,10 @@
         <v>82</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2">
         <v>70000</v>
@@ -1577,28 +1682,28 @@
         <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="G3" s="2">
         <v>700000</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="L3" s="2">
         <v>515</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="N3" s="2">
         <v>82</v>
@@ -1609,10 +1714,10 @@
         <v>83</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2">
         <v>50000</v>
@@ -1621,28 +1726,28 @@
         <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="G4" s="2">
         <v>500000</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="L4" s="2">
         <v>515</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="N4" s="2">
         <v>83</v>
@@ -1653,10 +1758,10 @@
         <v>84</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D5" s="2">
         <v>240000</v>
@@ -1665,28 +1770,28 @@
         <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="G5" s="2">
         <v>2400000</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="L5" s="2">
         <v>515</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="N5" s="2">
         <v>84</v>
@@ -1697,10 +1802,10 @@
         <v>85</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D6" s="2">
         <v>31274</v>
@@ -1709,28 +1814,28 @@
         <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="G6" s="2">
         <v>312740</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="L6" s="2">
         <v>515</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="N6" s="2">
         <v>85</v>
@@ -1741,10 +1846,10 @@
         <v>86</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D7" s="2">
         <v>250000</v>
@@ -1753,28 +1858,28 @@
         <v>10</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="G7" s="2">
         <v>2500000</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="L7" s="2">
         <v>515</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="N7" s="2">
         <v>86</v>
@@ -1785,10 +1890,10 @@
         <v>87</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D8" s="2">
         <v>200000</v>
@@ -1797,28 +1902,28 @@
         <v>10</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="G8" s="2">
         <v>2000000</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="L8" s="2">
         <v>515</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="N8" s="2">
         <v>87</v>
@@ -1829,10 +1934,10 @@
         <v>88</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D9" s="2">
         <v>115000</v>
@@ -1841,28 +1946,28 @@
         <v>10</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="G9" s="2">
         <v>1150000</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="L9" s="2">
         <v>515</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="N9" s="2">
         <v>88</v>
@@ -1873,10 +1978,10 @@
         <v>89</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D10" s="2">
         <v>40000</v>
@@ -1885,28 +1990,28 @@
         <v>10</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="G10" s="2">
         <v>400000</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="L10" s="2">
         <v>515</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="N10" s="2">
         <v>89</v>
@@ -1917,10 +2022,10 @@
         <v>90</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2">
         <v>48000</v>
@@ -1929,28 +2034,28 @@
         <v>10</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="G11" s="2">
         <v>480000</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="L11" s="2">
         <v>515</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="N11" s="2">
         <v>90</v>
@@ -1971,16 +2076,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1988,13 +2093,13 @@
         <v>110</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C2" s="2">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E2" s="2">
         <v>600000</v>
@@ -2005,13 +2110,13 @@
         <v>111</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C3" s="2">
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E3" s="2">
         <v>2000000</v>
@@ -2032,16 +2137,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2049,16 +2154,16 @@
         <v>116</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2066,16 +2171,16 @@
         <v>117</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2083,16 +2188,16 @@
         <v>118</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2100,16 +2205,16 @@
         <v>119</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2117,16 +2222,16 @@
         <v>120</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2144,22 +2249,22 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2167,22 +2272,22 @@
         <v>130</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E2" s="2">
         <v>21113089</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2190,22 +2295,22 @@
         <v>131</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E3" s="2">
         <v>9650048</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2223,22 +2328,22 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2246,7 +2351,7 @@
         <v>136</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>125</v>
@@ -2269,7 +2374,7 @@
         <v>137</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>125</v>

</xml_diff>

<commit_message>
#5: property boat&car done
</commit_message>
<xml_diff>
--- a/legislator/property/output/normal/丁守中_2011-11-22_財產申報表_tmp8fef1.xlsx
+++ b/legislator/property/output/normal/丁守中_2011-11-22_財產申報表_tmp8fef1.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="100">
   <si>
     <t>name</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>93年08月19曰</t>
+  </si>
+  <si>
+    <t>capacity</t>
   </si>
   <si>
     <t>LEXUSES350</t>
@@ -1333,38 +1336,59 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:14">
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1">
-        <v>3456</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" s="1">
-        <v>600000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="1">
         <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C2" s="2">
         <v>3456</v>
@@ -1373,13 +1397,34 @@
         <v>24</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G2" s="2">
         <v>600000</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="2">
+        <v>515</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="2">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1397,13 +1442,13 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>23</v>
@@ -1418,13 +1463,13 @@
         <v>61</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>23</v>
@@ -1439,13 +1484,13 @@
         <v>62</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>23</v>
@@ -1460,13 +1505,13 @@
         <v>63</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>23</v>
@@ -1481,13 +1526,13 @@
         <v>64</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>24</v>
@@ -1502,13 +1547,13 @@
         <v>65</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>24</v>
@@ -1523,13 +1568,13 @@
         <v>66</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>24</v>
@@ -1546,13 +1591,13 @@
         <v>67</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>24</v>
@@ -1567,13 +1612,13 @@
         <v>68</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>24</v>
@@ -1588,16 +1633,16 @@
         <v>70</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2">
@@ -1609,13 +1654,13 @@
         <v>71</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>24</v>
@@ -1630,13 +1675,13 @@
         <v>72</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>23</v>
@@ -1651,13 +1696,13 @@
         <v>73</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>24</v>
@@ -1672,13 +1717,13 @@
         <v>74</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>24</v>
@@ -1709,13 +1754,13 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>15</v>
@@ -1747,7 +1792,7 @@
         <v>81</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>24</v>
@@ -1759,13 +1804,13 @@
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G2" s="2">
         <v>16445990</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>34</v>
@@ -1791,7 +1836,7 @@
         <v>82</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>24</v>
@@ -1803,13 +1848,13 @@
         <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G3" s="2">
         <v>700000</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>34</v>
@@ -1835,7 +1880,7 @@
         <v>83</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>24</v>
@@ -1847,13 +1892,13 @@
         <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G4" s="2">
         <v>500000</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>34</v>
@@ -1879,7 +1924,7 @@
         <v>84</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>23</v>
@@ -1891,13 +1936,13 @@
         <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G5" s="2">
         <v>2400000</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>34</v>
@@ -1923,7 +1968,7 @@
         <v>85</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>23</v>
@@ -1935,13 +1980,13 @@
         <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G6" s="2">
         <v>312740</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>34</v>
@@ -1967,7 +2012,7 @@
         <v>86</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>24</v>
@@ -1979,13 +2024,13 @@
         <v>10</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G7" s="2">
         <v>2500000</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>34</v>
@@ -2011,7 +2056,7 @@
         <v>87</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>23</v>
@@ -2023,13 +2068,13 @@
         <v>10</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G8" s="2">
         <v>2000000</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>34</v>
@@ -2055,7 +2100,7 @@
         <v>88</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>23</v>
@@ -2067,13 +2112,13 @@
         <v>10</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G9" s="2">
         <v>1150000</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>34</v>
@@ -2099,7 +2144,7 @@
         <v>89</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>24</v>
@@ -2111,13 +2156,13 @@
         <v>10</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G10" s="2">
         <v>400000</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>34</v>
@@ -2143,7 +2188,7 @@
         <v>90</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>24</v>
@@ -2155,13 +2200,13 @@
         <v>10</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G11" s="2">
         <v>480000</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>34</v>
@@ -2197,7 +2242,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C1" s="1">
         <v>2</v>
@@ -2214,7 +2259,7 @@
         <v>110</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C2" s="2">
         <v>2</v>
@@ -2231,7 +2276,7 @@
         <v>111</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C3" s="2">
         <v>3</v>
@@ -2258,16 +2303,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2275,16 +2320,16 @@
         <v>116</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2292,16 +2337,16 @@
         <v>117</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2309,16 +2354,16 @@
         <v>118</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2326,16 +2371,16 @@
         <v>119</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2343,16 +2388,16 @@
         <v>120</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2370,22 +2415,22 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1">
         <v>21113089</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2393,22 +2438,22 @@
         <v>130</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E2" s="2">
         <v>21113089</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2416,22 +2461,22 @@
         <v>131</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E3" s="2">
         <v>9650048</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2452,19 +2497,19 @@
         <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E1" s="1">
         <v>990000</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2475,19 +2520,19 @@
         <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E2" s="2">
         <v>990000</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2495,22 +2540,22 @@
         <v>137</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E3" s="2">
         <v>2940000</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#5: property aircraft done
</commit_message>
<xml_diff>
--- a/legislator/property/output/normal/丁守中_2011-11-22_財產申報表_tmp8fef1.xlsx
+++ b/legislator/property/output/normal/丁守中_2011-11-22_財產申報表_tmp8fef1.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="102">
   <si>
     <t>name</t>
   </si>
@@ -162,6 +162,9 @@
     <t>93年08月19曰</t>
   </si>
   <si>
+    <t>building</t>
+  </si>
+  <si>
     <t>capacity</t>
   </si>
   <si>
@@ -172,6 +175,9 @@
   </si>
   <si>
     <t>貝賣</t>
+  </si>
+  <si>
+    <t>car</t>
   </si>
   <si>
     <t>台北富邦商業銀行</t>
@@ -1037,7 +1043,7 @@
         <v>31</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>34</v>
@@ -1090,7 +1096,7 @@
         <v>31</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>34</v>
@@ -1143,7 +1149,7 @@
         <v>31</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>34</v>
@@ -1196,7 +1202,7 @@
         <v>31</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>34</v>
@@ -1249,7 +1255,7 @@
         <v>31</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>34</v>
@@ -1302,7 +1308,7 @@
         <v>31</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>34</v>
@@ -1347,7 +1353,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1388,7 +1394,7 @@
         <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C2" s="2">
         <v>3456</v>
@@ -1397,16 +1403,16 @@
         <v>24</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G2" s="2">
         <v>600000</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>34</v>
@@ -1442,13 +1448,13 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>23</v>
@@ -1463,13 +1469,13 @@
         <v>61</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>23</v>
@@ -1484,13 +1490,13 @@
         <v>62</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>23</v>
@@ -1505,13 +1511,13 @@
         <v>63</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>23</v>
@@ -1526,13 +1532,13 @@
         <v>64</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>24</v>
@@ -1547,13 +1553,13 @@
         <v>65</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>24</v>
@@ -1568,13 +1574,13 @@
         <v>66</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>24</v>
@@ -1591,13 +1597,13 @@
         <v>67</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>24</v>
@@ -1612,13 +1618,13 @@
         <v>68</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>24</v>
@@ -1633,16 +1639,16 @@
         <v>70</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2">
@@ -1654,13 +1660,13 @@
         <v>71</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>24</v>
@@ -1675,13 +1681,13 @@
         <v>72</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>23</v>
@@ -1696,13 +1702,13 @@
         <v>73</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>24</v>
@@ -1717,13 +1723,13 @@
         <v>74</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>24</v>
@@ -1754,13 +1760,13 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>15</v>
@@ -1792,7 +1798,7 @@
         <v>81</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>24</v>
@@ -1804,13 +1810,13 @@
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G2" s="2">
         <v>16445990</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>34</v>
@@ -1836,7 +1842,7 @@
         <v>82</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>24</v>
@@ -1848,13 +1854,13 @@
         <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G3" s="2">
         <v>700000</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>34</v>
@@ -1880,7 +1886,7 @@
         <v>83</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>24</v>
@@ -1892,13 +1898,13 @@
         <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G4" s="2">
         <v>500000</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>34</v>
@@ -1924,7 +1930,7 @@
         <v>84</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>23</v>
@@ -1936,13 +1942,13 @@
         <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G5" s="2">
         <v>2400000</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>34</v>
@@ -1968,7 +1974,7 @@
         <v>85</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>23</v>
@@ -1980,13 +1986,13 @@
         <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G6" s="2">
         <v>312740</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>34</v>
@@ -2012,7 +2018,7 @@
         <v>86</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>24</v>
@@ -2024,13 +2030,13 @@
         <v>10</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G7" s="2">
         <v>2500000</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>34</v>
@@ -2056,7 +2062,7 @@
         <v>87</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>23</v>
@@ -2068,13 +2074,13 @@
         <v>10</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G8" s="2">
         <v>2000000</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>34</v>
@@ -2100,7 +2106,7 @@
         <v>88</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>23</v>
@@ -2112,13 +2118,13 @@
         <v>10</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G9" s="2">
         <v>1150000</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>34</v>
@@ -2144,7 +2150,7 @@
         <v>89</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>24</v>
@@ -2156,13 +2162,13 @@
         <v>10</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G10" s="2">
         <v>400000</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>34</v>
@@ -2188,7 +2194,7 @@
         <v>90</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>24</v>
@@ -2200,13 +2206,13 @@
         <v>10</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G11" s="2">
         <v>480000</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>34</v>
@@ -2242,7 +2248,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C1" s="1">
         <v>2</v>
@@ -2259,7 +2265,7 @@
         <v>110</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C2" s="2">
         <v>2</v>
@@ -2276,7 +2282,7 @@
         <v>111</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C3" s="2">
         <v>3</v>
@@ -2303,16 +2309,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2320,16 +2326,16 @@
         <v>116</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2337,16 +2343,16 @@
         <v>117</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2354,16 +2360,16 @@
         <v>118</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2371,16 +2377,16 @@
         <v>119</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2388,16 +2394,16 @@
         <v>120</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2415,22 +2421,22 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E1" s="1">
         <v>21113089</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2438,22 +2444,22 @@
         <v>130</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E2" s="2">
         <v>21113089</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2461,22 +2467,22 @@
         <v>131</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E3" s="2">
         <v>9650048</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2497,19 +2503,19 @@
         <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E1" s="1">
         <v>990000</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2520,19 +2526,19 @@
         <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E2" s="2">
         <v>990000</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2540,22 +2546,22 @@
         <v>137</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E3" s="2">
         <v>2940000</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#5: cash & deposit done
</commit_message>
<xml_diff>
--- a/legislator/property/output/normal/丁守中_2011-11-22_財產申報表_tmp8fef1.xlsx
+++ b/legislator/property/output/normal/丁守中_2011-11-22_財產申報表_tmp8fef1.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="105">
   <si>
     <t>name</t>
   </si>
@@ -180,42 +180,51 @@
     <t>car</t>
   </si>
   <si>
+    <t>bank</t>
+  </si>
+  <si>
+    <t>deposit_type</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
     <t>台北富邦商業銀行</t>
   </si>
   <si>
+    <t>中華郵政股份有限公司</t>
+  </si>
+  <si>
+    <t>永豐商業銀行</t>
+  </si>
+  <si>
+    <t>上海商業儲蓄銀行</t>
+  </si>
+  <si>
+    <t>國泰世華商業銀行</t>
+  </si>
+  <si>
+    <t>華南商業銀行信託部</t>
+  </si>
+  <si>
+    <t>兆豐國際商業銀行總管理處</t>
+  </si>
+  <si>
     <t>活期儲蓄存款</t>
   </si>
   <si>
+    <t>活期存款</t>
+  </si>
+  <si>
+    <t>定期存款</t>
+  </si>
+  <si>
+    <t>支票存款</t>
+  </si>
+  <si>
     <t>新臺幣</t>
   </si>
   <si>
-    <t>中華郵政股份有限公司</t>
-  </si>
-  <si>
-    <t>永豐商業銀行</t>
-  </si>
-  <si>
-    <t>上海商業儲蓄銀行</t>
-  </si>
-  <si>
-    <t>國泰世華商業銀行</t>
-  </si>
-  <si>
-    <t>華南商業銀行信託部</t>
-  </si>
-  <si>
-    <t>兆豐國際商業銀行總管理處</t>
-  </si>
-  <si>
-    <t>活期存款</t>
-  </si>
-  <si>
-    <t>定期存款</t>
-  </si>
-  <si>
-    <t>支票存款</t>
-  </si>
-  <si>
     <t>新臺幣t</t>
   </si>
   <si>
@@ -225,13 +234,13 @@
     <t>丁〇豪</t>
   </si>
   <si>
+    <t>deposit</t>
+  </si>
+  <si>
     <t>quantity</t>
   </si>
   <si>
     <t>face_value</t>
-  </si>
-  <si>
-    <t>currency</t>
   </si>
   <si>
     <t>琉園股份有限公司</t>
@@ -1440,13 +1449,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:13">
       <c r="B1" s="1" t="s">
         <v>52</v>
       </c>
@@ -1457,286 +1466,564 @@
         <v>54</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1">
-        <v>902545</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="1">
         <v>61</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2">
+      <c r="F2" s="2">
         <v>902545</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="G2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="2">
+        <v>515</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="1">
         <v>62</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2">
+      <c r="F3" s="2">
         <v>244533</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="G3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="2">
+        <v>515</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" s="2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="1">
         <v>63</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2">
+      <c r="F4" s="2">
         <v>201037</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="G4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="2">
+        <v>515</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="1">
         <v>64</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2">
+      <c r="F5" s="2">
         <v>2351650</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="G5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="2">
+        <v>515</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" s="2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="1">
         <v>65</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2">
+      <c r="F6" s="2">
         <v>115445</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="G6" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="2">
+        <v>515</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" s="2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="1">
         <v>66</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F7" s="2">
-        <v>20468.96</v>
-      </c>
-      <c r="G7" s="2">
         <v>612635.97</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="G7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="2">
+        <v>515</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" s="2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="1">
         <v>67</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2">
+      <c r="F8" s="2">
         <v>10000</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="G8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="2">
+        <v>515</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M8" s="2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="1">
         <v>68</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2">
+      <c r="F9" s="2">
         <v>505</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="G9" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="2">
+        <v>515</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M9" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="1">
         <v>70</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2">
+        <v>69</v>
+      </c>
+      <c r="F10" s="2">
         <v>274299</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="G10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="2">
+        <v>515</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="1">
         <v>71</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2">
+      <c r="F11" s="2">
         <v>55058</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="G11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="2">
+        <v>515</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M11" s="2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="1">
         <v>72</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2">
+      <c r="F12" s="2">
         <v>46287</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="G12" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="2">
+        <v>515</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M12" s="2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="1">
         <v>73</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2">
+      <c r="F13" s="2">
         <v>394133</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="G13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="2">
+        <v>515</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M13" s="2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="1">
         <v>74</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2">
+      <c r="F14" s="2">
         <v>197902</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" s="2">
+        <v>515</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M14" s="2">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1760,13 +2047,13 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>15</v>
@@ -1798,7 +2085,7 @@
         <v>81</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>24</v>
@@ -1810,13 +2097,13 @@
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="G2" s="2">
         <v>16445990</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>34</v>
@@ -1842,7 +2129,7 @@
         <v>82</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>24</v>
@@ -1854,13 +2141,13 @@
         <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="G3" s="2">
         <v>700000</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>34</v>
@@ -1886,7 +2173,7 @@
         <v>83</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>24</v>
@@ -1898,13 +2185,13 @@
         <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="G4" s="2">
         <v>500000</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>34</v>
@@ -1930,7 +2217,7 @@
         <v>84</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>23</v>
@@ -1942,13 +2229,13 @@
         <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="G5" s="2">
         <v>2400000</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>34</v>
@@ -1974,7 +2261,7 @@
         <v>85</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>23</v>
@@ -1986,13 +2273,13 @@
         <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="G6" s="2">
         <v>312740</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>34</v>
@@ -2018,7 +2305,7 @@
         <v>86</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>24</v>
@@ -2030,13 +2317,13 @@
         <v>10</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="G7" s="2">
         <v>2500000</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>34</v>
@@ -2062,7 +2349,7 @@
         <v>87</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>23</v>
@@ -2074,13 +2361,13 @@
         <v>10</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="G8" s="2">
         <v>2000000</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>34</v>
@@ -2106,7 +2393,7 @@
         <v>88</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>23</v>
@@ -2118,13 +2405,13 @@
         <v>10</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="G9" s="2">
         <v>1150000</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>34</v>
@@ -2150,7 +2437,7 @@
         <v>89</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>24</v>
@@ -2162,13 +2449,13 @@
         <v>10</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="G10" s="2">
         <v>400000</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>34</v>
@@ -2194,7 +2481,7 @@
         <v>90</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>24</v>
@@ -2206,13 +2493,13 @@
         <v>10</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="G11" s="2">
         <v>480000</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>34</v>
@@ -2248,7 +2535,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1">
         <v>2</v>
@@ -2265,7 +2552,7 @@
         <v>110</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C2" s="2">
         <v>2</v>
@@ -2282,7 +2569,7 @@
         <v>111</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C3" s="2">
         <v>3</v>
@@ -2309,16 +2596,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2326,16 +2613,16 @@
         <v>116</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2343,16 +2630,16 @@
         <v>117</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2360,16 +2647,16 @@
         <v>118</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2377,16 +2664,16 @@
         <v>119</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2394,16 +2681,16 @@
         <v>120</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2421,22 +2708,22 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E1" s="1">
         <v>21113089</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2444,22 +2731,22 @@
         <v>130</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E2" s="2">
         <v>21113089</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2467,22 +2754,22 @@
         <v>131</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E3" s="2">
         <v>9650048</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2503,19 +2790,19 @@
         <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E1" s="1">
         <v>990000</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2526,19 +2813,19 @@
         <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E2" s="2">
         <v>990000</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2546,22 +2833,22 @@
         <v>137</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E3" s="2">
         <v>2940000</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#5: fund, bonds, otherbonds, antique done
</commit_message>
<xml_diff>
--- a/legislator/property/output/normal/丁守中_2011-11-22_財產申報表_tmp8fef1.xlsx
+++ b/legislator/property/output/normal/丁守中_2011-11-22_財產申報表_tmp8fef1.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="106">
   <si>
     <t>name</t>
   </si>
@@ -273,7 +273,10 @@
     <t>手錶</t>
   </si>
   <si>
-    <t>手錶珠寶■</t>
+    <t>手錶珠寶</t>
+  </si>
+  <si>
+    <t>otherbonds</t>
   </si>
   <si>
     <t>南山人壽</t>
@@ -2527,27 +2530,48 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="1">
-        <v>600000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>110</v>
       </c>
@@ -2563,8 +2587,29 @@
       <c r="E2" s="2">
         <v>600000</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="2">
+        <v>515</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" s="2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>111</v>
       </c>
@@ -2579,6 +2624,27 @@
       </c>
       <c r="E3" s="2">
         <v>2000000</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="2">
+        <v>515</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="2">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2596,16 +2662,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2613,16 +2679,16 @@
         <v>116</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2630,16 +2696,16 @@
         <v>117</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2647,16 +2713,16 @@
         <v>118</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2664,16 +2730,16 @@
         <v>119</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2681,16 +2747,16 @@
         <v>120</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>69</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2708,22 +2774,22 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E1" s="1">
         <v>21113089</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2731,22 +2797,22 @@
         <v>130</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E2" s="2">
         <v>21113089</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2754,22 +2820,22 @@
         <v>131</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E3" s="2">
         <v>9650048</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2790,19 +2856,19 @@
         <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E1" s="1">
         <v>990000</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2813,19 +2879,19 @@
         <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E2" s="2">
         <v>990000</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2836,19 +2902,19 @@
         <v>69</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E3" s="2">
         <v>2940000</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#5: insurance, claim, debt, investment done
</commit_message>
<xml_diff>
--- a/legislator/property/output/normal/丁守中_2011-11-22_財產申報表_tmp8fef1.xlsx
+++ b/legislator/property/output/normal/丁守中_2011-11-22_財產申報表_tmp8fef1.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="107">
   <si>
     <t>name</t>
   </si>
@@ -276,42 +276,39 @@
     <t>手錶珠寶</t>
   </si>
   <si>
-    <t>otherbonds</t>
+    <t>antique</t>
+  </si>
+  <si>
+    <t>company</t>
   </si>
   <si>
     <t>南山人壽</t>
   </si>
   <si>
+    <t>國泰人壽</t>
+  </si>
+  <si>
     <t>南山康福20年期終身壽險</t>
   </si>
   <si>
-    <t>20年期年繳68310元.</t>
-  </si>
-  <si>
-    <t>南.山人壽</t>
-  </si>
-  <si>
-    <t>國泰人壽</t>
-  </si>
-  <si>
     <t>終身壽險</t>
   </si>
   <si>
-    <t>2t)年期终身壽險年繳56167元</t>
-  </si>
-  <si>
-    <t>新20年期繳費特別增值分红年繳64602元</t>
-  </si>
-  <si>
-    <t>新2b年繳費特別增值分紅年繳41542元</t>
-  </si>
-  <si>
-    <t>终身壽險年繳55407元</t>
+    <t>insurance</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>debtor</t>
   </si>
   <si>
     <t>房犀十地抵押貸款</t>
   </si>
   <si>
+    <t>房岸十地抵押貸款</t>
+  </si>
+  <si>
     <t>華南銀行臺北市北投區北投路</t>
   </si>
   <si>
@@ -321,7 +318,10 @@
     <t>房屋土地抵押貸款</t>
   </si>
   <si>
-    <t>房岸十地抵押貸款</t>
+    <t>debt</t>
+  </si>
+  <si>
+    <t>address</t>
   </si>
   <si>
     <t>鼎天股份有限公司</t>
@@ -333,13 +333,16 @@
     <t>95年09月01日</t>
   </si>
   <si>
+    <t>97年02月01日</t>
+  </si>
+  <si>
     <t>投資</t>
   </si>
   <si>
-    <t>97年02月01日</t>
-  </si>
-  <si>
     <t>贈與</t>
+  </si>
+  <si>
+    <t>investment</t>
   </si>
 </sst>
 </file>
@@ -2654,109 +2657,217 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:11">
       <c r="B1" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>116</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>90</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="2">
+        <v>515</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>117</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>90</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="2">
+        <v>515</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="1">
         <v>118</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="2">
+        <v>515</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="1">
         <v>119</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>90</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="2">
+        <v>515</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" s="2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>120</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>69</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="2">
+        <v>515</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" s="2">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2766,76 +2877,139 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:14">
       <c r="B1" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>92</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E1" s="1">
-        <v>21113089</v>
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>97</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="1">
         <v>130</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="E2" s="2">
         <v>21113089</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="I2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="2">
+        <v>515</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="1">
         <v>131</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E3" s="2">
         <v>9650048</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>98</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="2">
+        <v>515</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="2">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2845,33 +3019,54 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:14">
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E1" s="1">
-        <v>990000</v>
+        <v>99</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>102</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="1">
         <v>136</v>
       </c>
@@ -2891,10 +3086,31 @@
         <v>102</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>104</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="2">
+        <v>515</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="1">
         <v>137</v>
       </c>
@@ -2911,10 +3127,31 @@
         <v>2940000</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>105</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="2">
+        <v>515</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="2">
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>